<commit_message>
man-hours breakdown, midterms slides (pdf)
</commit_message>
<xml_diff>
--- a/Documentation/MIDTERMS PPT SLIDES/Bug Metrics.xlsx
+++ b/Documentation/MIDTERMS PPT SLIDES/Bug Metrics.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teh Kaixin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teh Kaixin\Desktop\FYP GIT\Ulink\Documentation\MIDTERMS PPT SLIDES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="465" windowWidth="25515" windowHeight="15540" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="1785" yWindow="465" windowWidth="25515" windowHeight="15540" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Bug Score" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1597,33 +1597,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1661,12 +1634,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1688,20 +1655,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1715,9 +1673,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1748,6 +1703,51 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2444,542 +2444,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'Bug Log Iter 1-10'!$I$23:$I$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-64FC-41BA-923A-04850402F689}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'Bug Log Iter 1-10'!$J$23:$J$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-64FC-41BA-923A-04850402F689}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'Bug Log Iter 1-10'!$K$23:$K$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-64FC-41BA-923A-04850402F689}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'Bug Log Iter 1-10'!$L$23:$L$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-64FC-41BA-923A-04850402F689}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>'Bug Log Iter 1-10'!$M$23:$M$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-64FC-41BA-923A-04850402F689}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="1390875567"/>
-        <c:axId val="1390876399"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1390875567"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1390876399"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1390876399"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1390875567"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3020,552 +2484,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4265,36 +3184,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>61912</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>219075</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>252412</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
@@ -4316,7 +3205,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:srcRect r="66960" b="17381"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -4353,7 +3242,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4391,7 +3280,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4764,13 +3653,13 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="67">
+      <c r="A3" s="119">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="78">
+      <c r="C3" s="69">
         <v>3</v>
       </c>
       <c r="D3" s="6">
@@ -4791,11 +3680,11 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="67"/>
+      <c r="A4" s="119"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="78">
+      <c r="C4" s="69">
         <v>3</v>
       </c>
       <c r="D4" s="6">
@@ -4816,11 +3705,11 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="67"/>
+      <c r="A5" s="119"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="78">
+      <c r="C5" s="69">
         <v>3</v>
       </c>
       <c r="D5" s="6">
@@ -4841,11 +3730,11 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
+      <c r="A6" s="119"/>
       <c r="B6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="78">
+      <c r="C6" s="69">
         <v>3</v>
       </c>
       <c r="D6" s="9"/>
@@ -4857,11 +3746,11 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="67"/>
+      <c r="A7" s="119"/>
       <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="78">
+      <c r="C7" s="69">
         <v>2</v>
       </c>
       <c r="D7" s="3">
@@ -4880,11 +3769,11 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="67"/>
+      <c r="A8" s="119"/>
       <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="78">
+      <c r="C8" s="69">
         <v>1</v>
       </c>
       <c r="D8" s="3">
@@ -4903,11 +3792,11 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="67"/>
+      <c r="A9" s="119"/>
       <c r="B9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="78">
+      <c r="C9" s="69">
         <v>3</v>
       </c>
       <c r="D9" s="3">
@@ -4928,11 +3817,11 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="67"/>
+      <c r="A10" s="119"/>
       <c r="B10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="78">
+      <c r="C10" s="69">
         <v>6</v>
       </c>
       <c r="D10" s="8"/>
@@ -4952,14 +3841,14 @@
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="67"/>
-      <c r="B11" s="68" t="s">
+      <c r="A11" s="119"/>
+      <c r="B11" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="122"/>
       <c r="G11" s="13">
         <f>SUM(G3:G10)</f>
         <v>10</v>
@@ -4970,13 +3859,13 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="71">
+      <c r="A12" s="123">
         <v>3</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="79">
+      <c r="C12" s="70">
         <v>12</v>
       </c>
       <c r="D12" s="19" t="s">
@@ -4996,11 +3885,11 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="71"/>
+      <c r="A13" s="123"/>
       <c r="B13" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="79">
+      <c r="C13" s="70">
         <v>8</v>
       </c>
       <c r="D13" s="19">
@@ -5020,11 +3909,11 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="71"/>
+      <c r="A14" s="123"/>
       <c r="B14" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="79">
+      <c r="C14" s="70">
         <v>7</v>
       </c>
       <c r="D14" s="21" t="s">
@@ -5044,14 +3933,14 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="71"/>
-      <c r="B15" s="68" t="s">
+      <c r="A15" s="123"/>
+      <c r="B15" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="70"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="122"/>
       <c r="G15" s="13">
         <f>SUM(G12:G14)</f>
         <v>39</v>
@@ -5059,13 +3948,13 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="66">
+      <c r="A16" s="118">
         <v>6</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="79">
+      <c r="C16" s="70">
         <v>15</v>
       </c>
       <c r="D16" s="21">
@@ -5083,14 +3972,14 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="66"/>
-      <c r="B17" s="66" t="s">
+      <c r="A17" s="118"/>
+      <c r="B17" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
+      <c r="C17" s="118"/>
+      <c r="D17" s="118"/>
+      <c r="E17" s="118"/>
+      <c r="F17" s="118"/>
       <c r="G17" s="13">
         <f>SUM(G16)</f>
         <v>19</v>
@@ -5098,13 +3987,13 @@
       <c r="H17" s="20"/>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="66">
+      <c r="A20" s="118">
         <v>6</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="79">
+      <c r="C20" s="70">
         <v>15</v>
       </c>
       <c r="D20" s="64">
@@ -5122,14 +4011,14 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="66"/>
-      <c r="B21" s="66" t="s">
+      <c r="A21" s="118"/>
+      <c r="B21" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
+      <c r="C21" s="118"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="118"/>
       <c r="G21" s="13">
         <f>SUM(G20)</f>
         <v>19</v>
@@ -5147,7 +4036,7 @@
       <c r="H22" s="63"/>
     </row>
     <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="66">
+      <c r="A23" s="118">
         <v>8</v>
       </c>
       <c r="B23" s="25" t="s">
@@ -5171,7 +4060,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="66"/>
+      <c r="A24" s="118"/>
       <c r="B24" s="25" t="s">
         <v>206</v>
       </c>
@@ -5193,14 +4082,14 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="66"/>
-      <c r="B25" s="66" t="s">
+      <c r="A25" s="118"/>
+      <c r="B25" s="118" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="66"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="66"/>
+      <c r="C25" s="118"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="118"/>
+      <c r="F25" s="118"/>
       <c r="G25" s="13">
         <f>SUM(G23:G24)</f>
         <v>26</v>
@@ -5234,7 +4123,7 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -6109,10 +4998,10 @@
         <v>87</v>
       </c>
       <c r="D27" s="30"/>
-      <c r="E27" s="72" t="s">
+      <c r="E27" s="124" t="s">
         <v>100</v>
       </c>
-      <c r="F27" s="72"/>
+      <c r="F27" s="124"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -6324,7 +5213,7 @@
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="L36" s="73" t="s">
+      <c r="L36" s="125" t="s">
         <v>203</v>
       </c>
     </row>
@@ -6358,7 +5247,7 @@
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="73"/>
+      <c r="L37" s="125"/>
     </row>
     <row r="38" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
@@ -6390,7 +5279,7 @@
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="73"/>
+      <c r="L38" s="125"/>
     </row>
     <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
@@ -6422,7 +5311,7 @@
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="73"/>
+      <c r="L39" s="125"/>
     </row>
     <row r="40" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
@@ -6454,7 +5343,7 @@
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="73"/>
+      <c r="L40" s="125"/>
     </row>
     <row r="41" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
@@ -6486,7 +5375,7 @@
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="73"/>
+      <c r="L41" s="125"/>
     </row>
     <row r="42" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
@@ -6518,7 +5407,7 @@
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-      <c r="L42" s="73"/>
+      <c r="L42" s="125"/>
     </row>
     <row r="43" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
@@ -6550,7 +5439,7 @@
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
-      <c r="L43" s="73"/>
+      <c r="L43" s="125"/>
     </row>
     <row r="44" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
@@ -6582,7 +5471,7 @@
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-      <c r="L44" s="73"/>
+      <c r="L44" s="125"/>
     </row>
     <row r="45" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
@@ -6612,7 +5501,7 @@
       <c r="K45" s="5">
         <v>42757</v>
       </c>
-      <c r="L45" s="73"/>
+      <c r="L45" s="125"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
@@ -7497,7 +6386,7 @@
       <c r="D74" s="30">
         <v>2</v>
       </c>
-      <c r="E74" s="74" t="s">
+      <c r="E74" s="126" t="s">
         <v>229</v>
       </c>
       <c r="F74" s="27" t="s">
@@ -7531,7 +6420,7 @@
       <c r="D75" s="30">
         <v>3</v>
       </c>
-      <c r="E75" s="74"/>
+      <c r="E75" s="126"/>
       <c r="F75" s="27" t="s">
         <v>223</v>
       </c>
@@ -8355,7 +7244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="L14:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -8395,8 +7284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G11" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8449,7 +7338,7 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="67">
+      <c r="A3" s="119">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -8458,14 +7347,14 @@
       <c r="C3" s="65">
         <v>1</v>
       </c>
-      <c r="D3" s="81">
+      <c r="D3" s="72">
         <v>0</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
       </c>
       <c r="F3" s="63">
-        <f>SUM(C3*$C$2,D3*$D$2,E3*$E$2)</f>
+        <f t="shared" ref="F3:F10" si="0">SUM(C3*$C$2,D3*$D$2,E3*$E$2)</f>
         <v>1</v>
       </c>
       <c r="G3" s="63" t="s">
@@ -8473,7 +7362,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="67"/>
+      <c r="A4" s="119"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
@@ -8485,7 +7374,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="63">
-        <f>SUM(C4*$C$2,D4*$D$2,E4*$E$2)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G4" s="63" t="s">
@@ -8493,7 +7382,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="67"/>
+      <c r="A5" s="119"/>
       <c r="B5" s="12" t="s">
         <v>13</v>
       </c>
@@ -8507,7 +7396,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="63">
-        <f>SUM(C5*$C$2,D5*$D$2,E5*$E$2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G5" s="63" t="s">
@@ -8515,7 +7404,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
+      <c r="A6" s="119"/>
       <c r="B6" s="12" t="s">
         <v>32</v>
       </c>
@@ -8525,7 +7414,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="63">
-        <f>SUM(C6*$C$2,D6*$D$2,E6*$E$2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G6" s="63" t="s">
@@ -8533,7 +7422,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="67"/>
+      <c r="A7" s="119"/>
       <c r="B7" s="12" t="s">
         <v>14</v>
       </c>
@@ -8545,7 +7434,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="63">
-        <f>SUM(C7*$C$2,D7*$D$2,E7*$E$2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G7" s="63" t="s">
@@ -8553,7 +7442,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="67"/>
+      <c r="A8" s="119"/>
       <c r="B8" s="12" t="s">
         <v>15</v>
       </c>
@@ -8565,7 +7454,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="63">
-        <f>SUM(C8*$C$2,D8*$D$2,E8*$E$2)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G8" s="63" t="s">
@@ -8573,7 +7462,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="67"/>
+      <c r="A9" s="119"/>
       <c r="B9" s="12" t="s">
         <v>33</v>
       </c>
@@ -8587,7 +7476,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="63">
-        <f>SUM(C9*$C$2,D9*$D$2,E9*$E$2)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G9" s="63" t="s">
@@ -8595,52 +7484,52 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="67"/>
-      <c r="B10" s="98" t="s">
+      <c r="A10" s="119"/>
+      <c r="B10" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="85">
+      <c r="C10" s="76">
         <v>3</v>
       </c>
-      <c r="D10" s="86"/>
-      <c r="E10" s="87"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="78"/>
       <c r="F10" s="63">
-        <f>SUM(C10*$C$2,D10*$D$2,E10*$E$2)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G10" s="63"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="97"/>
-      <c r="B11" s="100" t="s">
+      <c r="A11" s="128"/>
+      <c r="B11" s="87" t="s">
         <v>277</v>
       </c>
-      <c r="C11" s="90">
+      <c r="C11" s="79">
         <f>SUM(C3:C10)</f>
         <v>12</v>
       </c>
-      <c r="D11" s="91">
+      <c r="D11" s="80">
         <f>SUM(D3:D10)*5</f>
         <v>5</v>
       </c>
-      <c r="E11" s="92">
+      <c r="E11" s="81">
         <f>SUM(E3:E10)*10</f>
         <v>0</v>
       </c>
-      <c r="F11" s="84"/>
+      <c r="F11" s="75"/>
       <c r="G11" s="63" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="67"/>
-      <c r="B12" s="99" t="s">
+      <c r="A12" s="119"/>
+      <c r="B12" s="129" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="89"/>
-      <c r="F12" s="80">
+      <c r="C12" s="130"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="71">
         <f>SUM(F3:F10)</f>
         <v>17</v>
       </c>
@@ -8650,7 +7539,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="71">
+      <c r="A13" s="123">
         <v>3</v>
       </c>
       <c r="B13" s="17" t="s">
@@ -8674,7 +7563,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="71"/>
+      <c r="A14" s="123"/>
       <c r="B14" s="17" t="s">
         <v>40</v>
       </c>
@@ -8688,7 +7577,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="64">
-        <f t="shared" ref="F14:F15" si="0">SUM(C14*$C$2,D14*$D$2,E14*$E$2)</f>
+        <f t="shared" ref="F14:F15" si="1">SUM(C14*$C$2,D14*$D$2,E14*$E$2)</f>
         <v>2</v>
       </c>
       <c r="G14" s="64" t="s">
@@ -8696,21 +7585,21 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="71"/>
-      <c r="B15" s="102" t="s">
+      <c r="A15" s="123"/>
+      <c r="B15" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="93">
+      <c r="C15" s="82">
         <v>3</v>
       </c>
-      <c r="D15" s="93">
+      <c r="D15" s="82">
         <v>0</v>
       </c>
-      <c r="E15" s="93">
+      <c r="E15" s="82">
         <v>0</v>
       </c>
       <c r="F15" s="64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G15" s="22" t="s">
@@ -8718,53 +7607,53 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="101"/>
-      <c r="B16" s="103" t="s">
+      <c r="A16" s="132"/>
+      <c r="B16" s="89" t="s">
         <v>277</v>
       </c>
-      <c r="C16" s="94">
+      <c r="C16" s="83">
         <f>SUM(C13:C15)</f>
         <v>7</v>
       </c>
-      <c r="D16" s="95">
+      <c r="D16" s="84">
         <f>SUM(D13:D15)*5</f>
         <v>5</v>
       </c>
-      <c r="E16" s="96">
+      <c r="E16" s="85">
         <f>SUM(E13:E15)*10</f>
         <v>0</v>
       </c>
-      <c r="F16" s="83"/>
+      <c r="F16" s="74"/>
       <c r="G16" s="22"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
-      <c r="B17" s="99" t="s">
+      <c r="A17" s="123"/>
+      <c r="B17" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="89"/>
-      <c r="F17" s="80">
+      <c r="C17" s="130"/>
+      <c r="D17" s="130"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="71">
         <f>SUM(F13:F15)</f>
         <v>12</v>
       </c>
       <c r="G17" s="63"/>
     </row>
     <row r="18" spans="1:18" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="66">
+      <c r="A18" s="118">
         <v>6</v>
       </c>
-      <c r="B18" s="108" t="s">
+      <c r="B18" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="93">
+      <c r="C18" s="82">
         <v>4</v>
       </c>
-      <c r="D18" s="93">
+      <c r="D18" s="82">
         <v>2</v>
       </c>
-      <c r="E18" s="102">
+      <c r="E18" s="88">
         <v>2</v>
       </c>
       <c r="F18" s="64">
@@ -8779,60 +7668,60 @@
       </c>
     </row>
     <row r="19" spans="1:18" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="68"/>
-      <c r="B19" s="110" t="s">
+      <c r="A19" s="120"/>
+      <c r="B19" s="95" t="s">
         <v>277</v>
       </c>
-      <c r="C19" s="95">
+      <c r="C19" s="84">
         <f>C18</f>
         <v>4</v>
       </c>
-      <c r="D19" s="95">
+      <c r="D19" s="84">
         <f>D18*5</f>
         <v>10</v>
       </c>
-      <c r="E19" s="111">
+      <c r="E19" s="96">
         <f>10*E18</f>
         <v>20</v>
       </c>
-      <c r="F19" s="83"/>
+      <c r="F19" s="74"/>
       <c r="G19" s="22"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="66"/>
-      <c r="B20" s="109" t="s">
+      <c r="A20" s="118"/>
+      <c r="B20" s="127" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="109"/>
-      <c r="D20" s="109"/>
-      <c r="E20" s="109"/>
-      <c r="F20" s="80">
+      <c r="C20" s="127"/>
+      <c r="D20" s="127"/>
+      <c r="E20" s="127"/>
+      <c r="F20" s="71">
         <f>SUM(F18)</f>
         <v>34</v>
       </c>
       <c r="G20" s="63"/>
     </row>
     <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="118"/>
-      <c r="J21" s="112"/>
-      <c r="K21" s="112"/>
-      <c r="L21" s="112"/>
-      <c r="M21" s="119"/>
+      <c r="I21" s="103"/>
+      <c r="J21" s="97"/>
+      <c r="K21" s="97"/>
+      <c r="L21" s="97"/>
+      <c r="M21" s="104"/>
     </row>
     <row r="22" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="66">
+      <c r="A22" s="118">
         <v>7</v>
       </c>
-      <c r="B22" s="108" t="s">
+      <c r="B22" s="94" t="s">
         <v>275</v>
       </c>
-      <c r="C22" s="93">
+      <c r="C22" s="82">
         <v>3</v>
       </c>
-      <c r="D22" s="93">
+      <c r="D22" s="82">
         <v>2</v>
       </c>
-      <c r="E22" s="102">
+      <c r="E22" s="88">
         <v>1</v>
       </c>
       <c r="F22" s="64">
@@ -8842,78 +7731,78 @@
       <c r="G22" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="I22" s="129" t="s">
+      <c r="I22" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="130" t="s">
+      <c r="J22" s="115" t="s">
         <v>289</v>
       </c>
-      <c r="K22" s="131" t="s">
+      <c r="K22" s="116" t="s">
         <v>290</v>
       </c>
-      <c r="L22" s="132" t="s">
+      <c r="L22" s="117" t="s">
         <v>291</v>
       </c>
-      <c r="M22" s="129" t="s">
+      <c r="M22" s="114" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="68"/>
-      <c r="B23" s="110" t="s">
+      <c r="A23" s="120"/>
+      <c r="B23" s="95" t="s">
         <v>277</v>
       </c>
-      <c r="C23" s="95">
+      <c r="C23" s="84">
         <f>C22</f>
         <v>3</v>
       </c>
-      <c r="D23" s="95">
+      <c r="D23" s="84">
         <f>D22*5</f>
         <v>10</v>
       </c>
-      <c r="E23" s="111">
+      <c r="E23" s="96">
         <f>E22*10</f>
         <v>10</v>
       </c>
-      <c r="F23" s="83"/>
+      <c r="F23" s="74"/>
       <c r="G23" s="22"/>
-      <c r="I23" s="125">
+      <c r="I23" s="110">
         <v>2</v>
       </c>
-      <c r="J23" s="126">
+      <c r="J23" s="111">
         <f>C11</f>
         <v>12</v>
       </c>
-      <c r="K23" s="107">
+      <c r="K23" s="93">
         <f>D11</f>
         <v>5</v>
       </c>
-      <c r="L23" s="127">
+      <c r="L23" s="112">
         <f>E11</f>
         <v>0</v>
       </c>
-      <c r="M23" s="128">
+      <c r="M23" s="113">
         <f>F12</f>
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="66"/>
-      <c r="B24" s="109" t="s">
+      <c r="A24" s="118"/>
+      <c r="B24" s="127" t="s">
         <v>278</v>
       </c>
-      <c r="C24" s="109"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="80">
+      <c r="C24" s="127"/>
+      <c r="D24" s="127"/>
+      <c r="E24" s="127"/>
+      <c r="F24" s="71">
         <f>SUM(F22)</f>
         <v>23</v>
       </c>
       <c r="G24" s="63"/>
-      <c r="I24" s="106">
+      <c r="I24" s="92">
         <v>3</v>
       </c>
-      <c r="J24" s="105">
+      <c r="J24" s="91">
         <f>C16</f>
         <v>7</v>
       </c>
@@ -8921,32 +7810,32 @@
         <f>D16</f>
         <v>5</v>
       </c>
-      <c r="L24" s="104">
+      <c r="L24" s="90">
         <f>E16</f>
         <v>0</v>
       </c>
-      <c r="M24" s="82">
+      <c r="M24" s="73">
         <f>SUM(J24:L24)</f>
         <v>12</v>
       </c>
-      <c r="N24" s="112"/>
-      <c r="O24" s="112"/>
-      <c r="P24" s="112"/>
-      <c r="Q24" s="112"/>
-      <c r="R24" s="112"/>
+      <c r="N24" s="97"/>
+      <c r="O24" s="97"/>
+      <c r="P24" s="97"/>
+      <c r="Q24" s="97"/>
+      <c r="R24" s="97"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="75"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="76"/>
-      <c r="G25" s="77"/>
-      <c r="I25" s="106">
+      <c r="A25" s="66"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="68"/>
+      <c r="I25" s="92">
         <v>6</v>
       </c>
-      <c r="J25" s="105">
+      <c r="J25" s="91">
         <f>C19</f>
         <v>4</v>
       </c>
@@ -8954,22 +7843,22 @@
         <f>D19</f>
         <v>10</v>
       </c>
-      <c r="L25" s="104">
+      <c r="L25" s="90">
         <f>E19</f>
         <v>20</v>
       </c>
-      <c r="M25" s="82">
+      <c r="M25" s="73">
         <f>SUM(F20)</f>
         <v>34</v>
       </c>
-      <c r="N25" s="112"/>
-      <c r="O25" s="112"/>
-      <c r="P25" s="112"/>
-      <c r="Q25" s="112"/>
-      <c r="R25" s="112"/>
+      <c r="N25" s="97"/>
+      <c r="O25" s="97"/>
+      <c r="P25" s="97"/>
+      <c r="Q25" s="97"/>
+      <c r="R25" s="97"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="66">
+      <c r="A26" s="118">
         <v>8</v>
       </c>
       <c r="B26" s="25" t="s">
@@ -8991,10 +7880,10 @@
       <c r="G26" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="I26" s="106">
+      <c r="I26" s="92">
         <v>7</v>
       </c>
-      <c r="J26" s="105">
+      <c r="J26" s="91">
         <f>C23</f>
         <v>3</v>
       </c>
@@ -9002,22 +7891,22 @@
         <f>D23</f>
         <v>10</v>
       </c>
-      <c r="L26" s="104">
+      <c r="L26" s="90">
         <f>E23</f>
         <v>10</v>
       </c>
-      <c r="M26" s="82">
-        <f>SUM(J26:L26)</f>
+      <c r="M26" s="73">
+        <f t="shared" ref="M26:M32" si="2">SUM(J26:L26)</f>
         <v>23</v>
       </c>
-      <c r="N26" s="112"/>
-      <c r="O26" s="112"/>
-      <c r="P26" s="112"/>
-      <c r="Q26" s="112"/>
-      <c r="R26" s="112"/>
+      <c r="N26" s="97"/>
+      <c r="O26" s="97"/>
+      <c r="P26" s="97"/>
+      <c r="Q26" s="97"/>
+      <c r="R26" s="97"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="66"/>
+      <c r="A27" s="118"/>
       <c r="B27" s="25" t="s">
         <v>206</v>
       </c>
@@ -9037,10 +7926,10 @@
       <c r="G27" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="I27" s="106">
+      <c r="I27" s="92">
         <v>8</v>
       </c>
-      <c r="J27" s="105">
+      <c r="J27" s="91">
         <f>C28</f>
         <v>5</v>
       </c>
@@ -9048,22 +7937,22 @@
         <f>D28</f>
         <v>10</v>
       </c>
-      <c r="L27" s="104">
+      <c r="L27" s="90">
         <f>E28</f>
         <v>10</v>
       </c>
-      <c r="M27" s="82">
-        <f>SUM(J27:L27)</f>
+      <c r="M27" s="73">
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="N27" s="112"/>
-      <c r="O27" s="112"/>
-      <c r="P27" s="112"/>
-      <c r="Q27" s="112"/>
-      <c r="R27" s="112"/>
+      <c r="N27" s="97"/>
+      <c r="O27" s="97"/>
+      <c r="P27" s="97"/>
+      <c r="Q27" s="97"/>
+      <c r="R27" s="97"/>
     </row>
     <row r="28" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="66"/>
+      <c r="A28" s="118"/>
       <c r="B28" s="25" t="s">
         <v>277</v>
       </c>
@@ -9081,69 +7970,69 @@
       </c>
       <c r="F28" s="64"/>
       <c r="G28" s="64"/>
-      <c r="I28" s="113">
+      <c r="I28" s="98">
         <v>9</v>
       </c>
-      <c r="J28" s="114">
+      <c r="J28" s="99">
         <f>C33</f>
         <v>6</v>
       </c>
-      <c r="K28" s="115">
+      <c r="K28" s="100">
         <f>D33</f>
         <v>5</v>
       </c>
-      <c r="L28" s="116">
+      <c r="L28" s="101">
         <f>E33</f>
         <v>0</v>
       </c>
-      <c r="M28" s="117">
-        <f>SUM(J28:L28)</f>
+      <c r="M28" s="102">
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="N28" s="112"/>
-      <c r="O28" s="112"/>
-      <c r="P28" s="112"/>
-      <c r="Q28" s="112"/>
-      <c r="R28" s="112"/>
+      <c r="N28" s="97"/>
+      <c r="O28" s="97"/>
+      <c r="P28" s="97"/>
+      <c r="Q28" s="97"/>
+      <c r="R28" s="97"/>
     </row>
     <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="66"/>
-      <c r="B29" s="66" t="s">
+      <c r="A29" s="118"/>
+      <c r="B29" s="118" t="s">
         <v>279</v>
       </c>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="80">
+      <c r="C29" s="118"/>
+      <c r="D29" s="118"/>
+      <c r="E29" s="118"/>
+      <c r="F29" s="71">
         <f>SUM(F26:F27)</f>
         <v>25</v>
       </c>
       <c r="G29" s="63"/>
-      <c r="I29" s="120">
+      <c r="I29" s="105">
         <v>10</v>
       </c>
-      <c r="J29" s="121">
+      <c r="J29" s="106">
         <f>C39</f>
         <v>9</v>
       </c>
-      <c r="K29" s="122">
+      <c r="K29" s="107">
         <f>D39</f>
         <v>5</v>
       </c>
-      <c r="L29" s="123">
+      <c r="L29" s="108">
         <f>E39</f>
         <v>0</v>
       </c>
-      <c r="M29" s="124">
-        <f>SUM(J29:L29)</f>
+      <c r="M29" s="109">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I30" s="106">
+      <c r="I30" s="92">
         <v>8</v>
       </c>
-      <c r="J30" s="105">
+      <c r="J30" s="91">
         <f>C31</f>
         <v>2</v>
       </c>
@@ -9151,17 +8040,17 @@
         <f>D31</f>
         <v>1</v>
       </c>
-      <c r="L30" s="104">
+      <c r="L30" s="90">
         <f>E31</f>
         <v>0</v>
       </c>
-      <c r="M30" s="82">
-        <f>SUM(J30:L30)</f>
+      <c r="M30" s="73">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="66">
+      <c r="A31" s="118">
         <v>9</v>
       </c>
       <c r="B31" s="25" t="s">
@@ -9183,28 +8072,28 @@
       <c r="G31" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="I31" s="113">
+      <c r="I31" s="98">
         <v>9</v>
       </c>
-      <c r="J31" s="114">
+      <c r="J31" s="99">
         <f>C36</f>
         <v>1</v>
       </c>
-      <c r="K31" s="115">
+      <c r="K31" s="100">
         <f>D36</f>
         <v>0</v>
       </c>
-      <c r="L31" s="116">
+      <c r="L31" s="101">
         <f>E36</f>
         <v>0</v>
       </c>
-      <c r="M31" s="117">
-        <f>SUM(J31:L31)</f>
+      <c r="M31" s="102">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="66"/>
+      <c r="A32" s="118"/>
       <c r="B32" s="25" t="s">
         <v>284</v>
       </c>
@@ -9216,32 +8105,32 @@
         <v>0</v>
       </c>
       <c r="F32" s="64">
-        <f t="shared" ref="F32:F33" si="1">SUM(C32,D32*5,E32*10)</f>
+        <f t="shared" ref="F32" si="3">SUM(C32,D32*5,E32*10)</f>
         <v>2</v>
       </c>
       <c r="G32" s="22"/>
-      <c r="I32" s="120">
+      <c r="I32" s="105">
         <v>10</v>
       </c>
-      <c r="J32" s="121">
+      <c r="J32" s="106">
         <f>C42</f>
         <v>0</v>
       </c>
-      <c r="K32" s="122">
+      <c r="K32" s="107">
         <f>D42</f>
         <v>0</v>
       </c>
-      <c r="L32" s="123">
+      <c r="L32" s="108">
         <f>E42</f>
         <v>0</v>
       </c>
-      <c r="M32" s="124">
-        <f>SUM(J32:L32)</f>
+      <c r="M32" s="109">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="66"/>
+      <c r="A33" s="118"/>
       <c r="B33" s="25" t="s">
         <v>277</v>
       </c>
@@ -9262,21 +8151,21 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="66"/>
-      <c r="B34" s="66" t="s">
+      <c r="A34" s="118"/>
+      <c r="B34" s="118" t="s">
         <v>280</v>
       </c>
-      <c r="C34" s="66"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="66"/>
-      <c r="F34" s="80">
+      <c r="C34" s="118"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="118"/>
+      <c r="F34" s="71">
         <f>SUM(F31:F33)</f>
         <v>9</v>
       </c>
       <c r="G34" s="63"/>
     </row>
     <row r="36" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="66">
+      <c r="A36" s="118">
         <v>10</v>
       </c>
       <c r="B36" s="25" t="s">
@@ -9300,7 +8189,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="66"/>
+      <c r="A37" s="118"/>
       <c r="B37" s="25" t="s">
         <v>287</v>
       </c>
@@ -9314,7 +8203,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="64">
-        <f t="shared" ref="F37:F38" si="2">SUM(C37,D37*5,E37*10)</f>
+        <f t="shared" ref="F37:F38" si="4">SUM(C37,D37*5,E37*10)</f>
         <v>2</v>
       </c>
       <c r="G37" s="64" t="s">
@@ -9322,7 +8211,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="66"/>
+      <c r="A38" s="118"/>
       <c r="B38" s="25" t="s">
         <v>288</v>
       </c>
@@ -9336,13 +8225,13 @@
         <v>0</v>
       </c>
       <c r="F38" s="64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G38" s="64"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="66"/>
+      <c r="A39" s="118"/>
       <c r="B39" s="25" t="s">
         <v>285</v>
       </c>
@@ -9362,14 +8251,14 @@
       <c r="G39" s="64"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="66"/>
-      <c r="B40" s="66" t="s">
+      <c r="A40" s="118"/>
+      <c r="B40" s="118" t="s">
         <v>281</v>
       </c>
-      <c r="C40" s="66"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="66"/>
-      <c r="F40" s="80">
+      <c r="C40" s="118"/>
+      <c r="D40" s="118"/>
+      <c r="E40" s="118"/>
+      <c r="F40" s="71">
         <f>SUM(F36:F39)</f>
         <v>14</v>
       </c>
@@ -9377,6 +8266,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B20:E20"/>
     <mergeCell ref="A36:A40"/>
     <mergeCell ref="B40:E40"/>
     <mergeCell ref="A22:A24"/>
@@ -9385,12 +8280,6 @@
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="B34:E34"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B20:E20"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:E9 C11:E11 D10:E10">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">

</xml_diff>